<commit_message>
Revamped database functionality to be more versatile, allows access to data outside original Get...() functions through a global database Created a utilities folder for organizing utilities functions
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\MATLAB\DefinitiveTCM.git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\MATLAB\DefinitiveTCM.git\Utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="1" r:id="rId1"/>
+    <sheet name="Magnification" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,16 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Thermal Conductivity</t>
-  </si>
-  <si>
-    <t>Thermal Diffusion</t>
-  </si>
-  <si>
-    <t>Density</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>filmgold</t>
   </si>
@@ -57,6 +49,12 @@
   </si>
   <si>
     <t>material</t>
+  </si>
+  <si>
+    <t>magnification</t>
+  </si>
+  <si>
+    <t>spotsize</t>
   </si>
 </sst>
 </file>
@@ -384,11 +382,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,48 +398,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
+      <c r="B2">
+        <v>150</v>
+      </c>
+      <c r="C2" s="1">
+        <v>6.0718899999999999E-5</v>
+      </c>
+      <c r="D2">
+        <v>19300</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>150</v>
+        <v>1.089</v>
       </c>
       <c r="C3" s="1">
-        <v>6.0718899999999999E-5</v>
+        <v>6.5000000000000002E-7</v>
       </c>
       <c r="D3">
-        <v>19300</v>
+        <v>2530</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>318</v>
@@ -455,29 +455,15 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>1.089</v>
+        <v>6.5</v>
       </c>
       <c r="C5" s="1">
-        <v>6.5000000000000002E-7</v>
+        <v>3.3113999999999999E-7</v>
       </c>
       <c r="D5">
-        <v>2530</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>6.5</v>
-      </c>
-      <c r="C6" s="1">
-        <v>3.3113999999999999E-7</v>
-      </c>
-      <c r="D6">
         <v>2649</v>
       </c>
     </row>
@@ -485,4 +471,59 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>50</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.9999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1">
+        <v>5.0000000000000004E-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2.0000000000000002E-5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed rough draft of GPIB Interface classes Added Lock-in Amp Time Constant table to database Added toggle in PositionSample.fig to change control from the computer to a joystick
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\MATLAB\DefinitiveTCM.git\Utilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\MATLAB\DefinitiveTCM.git\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Materials" sheetId="1" r:id="rId1"/>
-    <sheet name="Magnification" sheetId="2" r:id="rId2"/>
+    <sheet name="Magnification" sheetId="2" r:id="rId1"/>
+    <sheet name="Materials" sheetId="1" r:id="rId2"/>
+    <sheet name="SRS830TimeConstants" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>filmgold</t>
   </si>
@@ -55,6 +56,12 @@
   </si>
   <si>
     <t>spotsize</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>timeConstant</t>
   </si>
 </sst>
 </file>
@@ -98,10 +105,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="48" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,9 +390,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>50</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.9999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1">
+        <v>5.0000000000000004E-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2.0000000000000002E-5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
@@ -473,54 +538,186 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>50</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1.9999999999999999E-6</v>
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>20</v>
-      </c>
-      <c r="B3" s="1">
-        <v>5.0000000000000004E-6</v>
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>3.0000000000000001E-6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1E-4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2.9999999999999997E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="B5" s="1">
-        <v>2.0000000000000002E-5</v>
+      <c r="B7" s="3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" s="3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" s="3">
+        <v>30000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>